<commit_message>
Přesunutí JS, index - menu, patička, mapa, nový GIT repozitář
</commit_message>
<xml_diff>
--- a/prace.xlsx
+++ b/prace.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Datum</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Nalezení nové šablony webu, její stažení</t>
+  </si>
+  <si>
+    <t>Nová šablona - přesunutí JS, index - menu, patička, mapa, nový GIT repozitář</t>
   </si>
 </sst>
 </file>
@@ -91,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -110,6 +113,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,14 +449,14 @@
       </c>
       <c r="E1">
         <f>SUM(B1:B488)</f>
-        <v>11</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42831</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="8">
         <v>3</v>
       </c>
       <c r="C2" t="s">
@@ -461,7 +467,7 @@
       <c r="A3" s="1">
         <v>42836</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="8">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -472,7 +478,7 @@
       <c r="A4" s="1">
         <v>42847</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="8">
         <v>5</v>
       </c>
       <c r="C4" t="s">
@@ -483,7 +489,7 @@
       <c r="A5" s="1">
         <v>42848</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="8">
         <v>1</v>
       </c>
       <c r="C5" t="s">
@@ -494,11 +500,22 @@
       <c r="A6" s="1">
         <v>42878</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="8">
         <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42885</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stránka O mě, fonty pro všechny stránky
</commit_message>
<xml_diff>
--- a/prace.xlsx
+++ b/prace.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Datum</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Nová šablona - přesunutí JS, index - menu, patička, mapa, nový GIT repozitář</t>
+  </si>
+  <si>
+    <t>Index - rozvržení, texty, rozvržení bloků apod..</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +452,7 @@
       </c>
       <c r="E1">
         <f>SUM(B1:B488)</f>
-        <v>13.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -516,6 +519,22 @@
       </c>
       <c r="C7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42886</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pěkné URL bez PHP
</commit_message>
<xml_diff>
--- a/prace.xlsx
+++ b/prace.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Stránky různých služeb</t>
+  </si>
+  <si>
+    <t>Reservanto první nasazení, Nahrazení head, keywords, title, Odstraněny nepotřebné stránky, Kontrola správnosti odkazů, Footer a jeho nahrazení ve stránkách, Nasazeno PHP - jednotné menu, Styly, tránka služeb, galerie, 404</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
@@ -461,7 +464,7 @@
       </c>
       <c r="E1">
         <f>SUM(B1:B488)</f>
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -572,6 +575,17 @@
       </c>
       <c r="C11" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>42890</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oprava chybek po testovacím nasazení
</commit_message>
<xml_diff>
--- a/prace.xlsx
+++ b/prace.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Datum</t>
   </si>
@@ -59,13 +59,16 @@
   </si>
   <si>
     <t>Reservanto první nasazení, Nahrazení head, keywords, title, Odstraněny nepotřebné stránky, Kontrola správnosti odkazů, Footer a jeho nahrazení ve stránkách, Nasazeno PHP - jednotné menu, Styly, tránka služeb, galerie, 404</t>
+  </si>
+  <si>
+    <t>Nasazení na testovací WWW bujabeza, odladění nějakých chyb, náhled pro Jarču</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,8 +85,34 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +125,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -106,10 +140,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -127,12 +162,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +486,7 @@
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -459,19 +496,19 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="8">
         <f>SUM(B1:B488)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42831</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>3</v>
       </c>
       <c r="C2" t="s">
@@ -482,7 +519,7 @@
       <c r="A3" s="1">
         <v>42836</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -493,7 +530,7 @@
       <c r="A4" s="1">
         <v>42847</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>5</v>
       </c>
       <c r="C4" t="s">
@@ -504,7 +541,7 @@
       <c r="A5" s="1">
         <v>42848</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>1</v>
       </c>
       <c r="C5" t="s">
@@ -515,7 +552,7 @@
       <c r="A6" s="1">
         <v>42878</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>1</v>
       </c>
       <c r="C6" t="s">
@@ -526,7 +563,7 @@
       <c r="A7" s="1">
         <v>42885</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>2.5</v>
       </c>
       <c r="C7" t="s">
@@ -586,6 +623,17 @@
       </c>
       <c r="C12" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>42890</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oprava textů, úvod a fotky ve sliderech
</commit_message>
<xml_diff>
--- a/prace.xlsx
+++ b/prace.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Datum</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Nasazení na testovací WWW bujabeza, odladění nějakých chyb, náhled pro Jarču</t>
+  </si>
+  <si>
+    <t>Nové obrázky na index+parallax, doplnění textů</t>
   </si>
 </sst>
 </file>
@@ -472,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +504,7 @@
       </c>
       <c r="E1" s="8">
         <f>SUM(B1:B488)</f>
-        <v>27</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -574,7 +577,7 @@
       <c r="A8" s="1">
         <v>42886</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="7">
         <v>2.5</v>
       </c>
       <c r="C8" t="s">
@@ -585,7 +588,7 @@
       <c r="A9" s="1">
         <v>42887</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="7">
         <v>1.5</v>
       </c>
       <c r="C9" t="s">
@@ -596,7 +599,7 @@
       <c r="A10" s="1">
         <v>42889</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="7">
         <v>2</v>
       </c>
       <c r="C10" t="s">
@@ -607,7 +610,7 @@
       <c r="A11" s="1">
         <v>42889</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="7">
         <v>1.5</v>
       </c>
       <c r="C11" t="s">
@@ -618,7 +621,7 @@
       <c r="A12" s="1">
         <v>42890</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="7">
         <v>5</v>
       </c>
       <c r="C12" t="s">
@@ -629,12 +632,89 @@
       <c r="A13" s="1">
         <v>42890</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="7">
         <v>1</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>42893</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lepší response (logo pryč), mapa nezpůsobuje spodní scrollbar, rezervanto tlačítko otevírá konkrétní služby+nastavení reservanta, hezčí homepage slidery
</commit_message>
<xml_diff>
--- a/prace.xlsx
+++ b/prace.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Datum</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Opraveny a dodány texty, reservanto, lepší skrolování, homepage 3 nové slidery - fotky</t>
+  </si>
+  <si>
+    <t>Lepší response (logo pryč), mapa nezpůsobuje spodní scrollbar, rezervanto tlačítko otevírá konkrétní služby+nastavení reservanta, hezčí homepage slidery</t>
   </si>
 </sst>
 </file>
@@ -481,7 +484,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +510,7 @@
       </c>
       <c r="E1" s="8">
         <f>SUM(B1:B488)</f>
-        <v>30.5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -665,7 +668,15 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
+      <c r="A16" s="1">
+        <v>42899</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>

</xml_diff>

<commit_message>
Galerie, odstranění nepotřebných obrázků, dodání obrázků do služeb
</commit_message>
<xml_diff>
--- a/prace.xlsx
+++ b/prace.xlsx
@@ -13,8 +13,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Za zaplacení domény + hostingu</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Datum</t>
   </si>
@@ -71,13 +105,19 @@
   </si>
   <si>
     <t>Lepší response (logo pryč), mapa nezpůsobuje spodní scrollbar, rezervanto tlačítko otevírá konkrétní služby+nastavení reservanta, hezčí homepage slidery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wedos - objednání domény + hostingu, spuštění demo verze, </t>
+  </si>
+  <si>
+    <t>plus 483,-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +160,19 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -153,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -176,6 +229,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -480,11 +536,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,9 +549,10 @@
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
     <col min="3" max="3" width="155.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -510,10 +567,13 @@
       </c>
       <c r="E1" s="8">
         <f>SUM(B1:B488)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42831</v>
       </c>
@@ -524,7 +584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42836</v>
       </c>
@@ -535,7 +595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42847</v>
       </c>
@@ -546,7 +606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42848</v>
       </c>
@@ -557,7 +617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42878</v>
       </c>
@@ -568,7 +628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42885</v>
       </c>
@@ -579,7 +639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42886</v>
       </c>
@@ -590,7 +650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42887</v>
       </c>
@@ -601,7 +661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42889</v>
       </c>
@@ -612,7 +672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42889</v>
       </c>
@@ -623,7 +683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42890</v>
       </c>
@@ -634,7 +694,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42890</v>
       </c>
@@ -645,7 +705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42893</v>
       </c>
@@ -656,7 +716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42898</v>
       </c>
@@ -667,7 +727,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42899</v>
       </c>
@@ -678,52 +738,60 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>42901</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
@@ -741,5 +809,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Doplnění popisků galerie, singulár/plurál
</commit_message>
<xml_diff>
--- a/prace.xlsx
+++ b/prace.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Datum</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>plus 483,-</t>
+  </si>
+  <si>
+    <t>Inverzní logo, dodání kurzu, galerie, obrázky v seznamu služeb a jednotlivbých službách, ičo</t>
+  </si>
+  <si>
+    <t>Doplnění popisků galerie, singulár/plurál</t>
   </si>
 </sst>
 </file>
@@ -540,7 +546,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +573,7 @@
       </c>
       <c r="E1" s="8">
         <f>SUM(B1:B488)</f>
-        <v>32</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>20</v>
@@ -750,10 +756,26 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
+      <c r="A18" s="1">
+        <v>42906</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
+      <c r="A19" s="1">
+        <v>42908</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>

</xml_diff>

<commit_message>
Finální práce - favicon, odstranění TODO, API klíče restrikce, kontrola, dodělání galerie, nastavení rezervací, publish
</commit_message>
<xml_diff>
--- a/prace.xlsx
+++ b/prace.xlsx
@@ -19,7 +19,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="D23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Datum</t>
   </si>
@@ -117,13 +117,25 @@
   </si>
   <si>
     <t>Doplnění popisků galerie, singulár/plurál</t>
+  </si>
+  <si>
+    <t>Cena za hod.:</t>
+  </si>
+  <si>
+    <t>Celkem za web:</t>
+  </si>
+  <si>
+    <t>Finální práce - favicon, odstranění TODO, API klíče restrikce, kontrola, dodělání galerie, nastavení rezervací, publish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;Kč&quot;"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +191,15 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -212,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -235,9 +256,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -543,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,10 +578,11 @@
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
     <col min="3" max="3" width="155.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -573,13 +597,16 @@
       </c>
       <c r="E1" s="8">
         <f>SUM(B1:B488)</f>
-        <v>33.799999999999997</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42831</v>
       </c>
@@ -590,7 +617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42836</v>
       </c>
@@ -601,7 +628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42847</v>
       </c>
@@ -612,7 +639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42848</v>
       </c>
@@ -623,7 +650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42878</v>
       </c>
@@ -634,7 +661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42885</v>
       </c>
@@ -645,7 +672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42886</v>
       </c>
@@ -656,7 +683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42887</v>
       </c>
@@ -667,7 +694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42889</v>
       </c>
@@ -678,7 +705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42889</v>
       </c>
@@ -689,7 +716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42890</v>
       </c>
@@ -700,7 +727,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42890</v>
       </c>
@@ -711,7 +738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42893</v>
       </c>
@@ -722,7 +749,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42898</v>
       </c>
@@ -733,7 +760,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42899</v>
       </c>
@@ -744,7 +771,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42901</v>
       </c>
@@ -755,7 +782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42906</v>
       </c>
@@ -766,7 +793,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42908</v>
       </c>
@@ -777,43 +804,61 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>42933</v>
+      </c>
+      <c r="B20" s="7">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="12">
+        <f>E1*I1</f>
+        <v>14319.999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Odstranění rezervanta + oprava textů
</commit_message>
<xml_diff>
--- a/prace.xlsx
+++ b/prace.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,17 +9,17 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D23" authorId="0" shapeId="0">
+    <comment ref="D23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -29,7 +29,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Datum</t>
   </si>
@@ -126,16 +126,22 @@
   </si>
   <si>
     <t>Finální práce - favicon, odstranění TODO, API klíče restrikce, kontrola, dodělání galerie, nastavení rezervací, publish</t>
+  </si>
+  <si>
+    <t>Aktualizace cen, zrušení některých služeb</t>
+  </si>
+  <si>
+    <t>Odstranění online rezervace, upravení textů</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;Kč&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +269,8 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Chybně" xfId="1" builtinId="27"/>
+    <cellStyle name="normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -280,9 +286,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv sady Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kancelář">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -320,9 +326,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kancelář">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -354,10 +360,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,10 +394,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kancelář">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -565,14 +569,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
@@ -582,7 +586,7 @@
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="23.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -597,7 +601,7 @@
       </c>
       <c r="E1" s="8">
         <f>SUM(B1:B488)</f>
-        <v>35.799999999999997</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="G1" t="s">
         <v>23</v>
@@ -606,7 +610,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>42831</v>
       </c>
@@ -617,7 +621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>42836</v>
       </c>
@@ -628,7 +632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>42847</v>
       </c>
@@ -639,7 +643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>42848</v>
       </c>
@@ -650,7 +654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>42878</v>
       </c>
@@ -661,7 +665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>42885</v>
       </c>
@@ -672,7 +676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>42886</v>
       </c>
@@ -683,7 +687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>42887</v>
       </c>
@@ -694,7 +698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>42889</v>
       </c>
@@ -705,7 +709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>42889</v>
       </c>
@@ -716,7 +720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>42890</v>
       </c>
@@ -727,7 +731,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>42890</v>
       </c>
@@ -738,7 +742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>42893</v>
       </c>
@@ -749,7 +753,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>42898</v>
       </c>
@@ -760,7 +764,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>42899</v>
       </c>
@@ -771,7 +775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>42901</v>
       </c>
@@ -782,7 +786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>42906</v>
       </c>
@@ -793,7 +797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>42908</v>
       </c>
@@ -804,7 +808,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>42933</v>
       </c>
@@ -815,62 +819,78 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>43048</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>43130</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
       <c r="D22" s="11" t="s">
         <v>24</v>
       </c>
       <c r="E22" s="12">
         <f>E1*I1</f>
-        <v>14319.999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14919.999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="B23" s="7"/>
       <c r="D23" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="B26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="B32" s="7"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2">
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2">
       <c r="B34" s="7"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2">
       <c r="B35" s="7"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2">
       <c r="B36" s="7"/>
     </row>
   </sheetData>

</xml_diff>